<commit_message>
Generates 10 weeks of sheets
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,6 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Week 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Week 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Week 5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Week 6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Week 7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Week 8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Week 9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Week 10" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -438,6 +447,816 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Tuesday, June 27, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, June 28, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, June 29, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, June 30, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, July 01, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, August 29, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, August 30, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, August 31, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, September 01, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, September 02, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, July 04, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, July 05, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, July 06, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, July 07, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, July 08, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, July 11, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, July 12, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, July 13, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, July 14, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, July 15, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, July 18, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, July 19, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, July 20, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, July 21, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, July 22, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
           <t>Tuesday, July 25, 2023</t>
         </is>
       </c>
@@ -459,6 +1278,654 @@
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Saturday, July 29, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, August 01, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, August 02, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, August 03, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, August 04, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, August 05, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, August 08, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, August 09, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, August 10, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, August 11, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, August 12, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, August 15, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, August 16, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, August 17, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, August 18, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, August 19, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Arrival</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t># in Party</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday, August 22, 2023</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday, August 23, 2023</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Thursday, August 24, 2023</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Friday, August 25, 2023</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Saturday, August 26, 2023</t>
         </is>
       </c>
     </row>

</xml_diff>